<commit_message>
actualizacao da sessao 8 chimanimani
</commit_message>
<xml_diff>
--- a/desistentes.xlsx
+++ b/desistentes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -33,9 +33,15 @@
     <t>C_1152</t>
   </si>
   <si>
+    <t>C_1119</t>
+  </si>
+  <si>
     <t>C_1155</t>
   </si>
   <si>
+    <t>C_1096</t>
+  </si>
+  <si>
     <t>C_1145</t>
   </si>
   <si>
@@ -60,9 +66,15 @@
     <t>FILIPE KUGSTONE</t>
   </si>
   <si>
+    <t>GUERRA RAZAO</t>
+  </si>
+  <si>
     <t>JORGE MATEUS</t>
   </si>
   <si>
+    <t>MATEUS LUCAS KUMBI</t>
+  </si>
+  <si>
     <t>NOA MOISES HACHA</t>
   </si>
   <si>
@@ -87,6 +99,9 @@
     <t>GORONGOSA-NHAMU</t>
   </si>
   <si>
+    <t>CHIMANIMANI-MPUNGA</t>
+  </si>
+  <si>
     <t>Turma</t>
   </si>
   <si>
@@ -99,6 +114,9 @@
     <t>H_1</t>
   </si>
   <si>
+    <t>AP-6</t>
+  </si>
+  <si>
     <t>Membro_Influente</t>
   </si>
   <si>
@@ -108,13 +126,16 @@
     <t>NAO</t>
   </si>
   <si>
+    <t>SIM</t>
+  </si>
+  <si>
     <t>Tipo_influencia</t>
   </si>
   <si>
+    <t>FISCAL COMUNITARIO</t>
+  </si>
+  <si>
     <t>ProdutorLider</t>
-  </si>
-  <si>
-    <t>SIM</t>
   </si>
   <si>
     <t>Tempo_produtor</t>
@@ -197,7 +218,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S11"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -205,58 +226,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="L1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="M1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="N1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="O1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="Q1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="R1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -264,54 +285,54 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0"/>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J2" s="0"/>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N2" s="0">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -319,54 +340,54 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J3" s="0"/>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N3" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -374,54 +395,54 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J4" s="0"/>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N4" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="R4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="S4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -429,54 +450,54 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="0"/>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J5" s="0"/>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N5" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -484,54 +505,54 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J6" s="0"/>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N6" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R6" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -539,54 +560,54 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0"/>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N7" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="Q7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -594,54 +615,54 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N8" s="0">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="P8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="R8" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="S8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -649,54 +670,164 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="I9" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J9" s="0"/>
       <c r="K9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="L9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M9" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N9" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q9" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="R9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="S9" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0"/>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="0"/>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" s="0">
+        <v>2</v>
+      </c>
+      <c r="O10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>49</v>
+      </c>
+      <c r="R10" t="s">
+        <v>51</v>
+      </c>
+      <c r="S10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0"/>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="0"/>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" s="0">
+        <v>7</v>
+      </c>
+      <c r="O11" t="s">
+        <v>36</v>
+      </c>
+      <c r="P11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>35</v>
+      </c>
+      <c r="R11" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacao das base de dados
</commit_message>
<xml_diff>
--- a/desistentes.xlsx
+++ b/desistentes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -27,6 +27,9 @@
     <t>C_1034</t>
   </si>
   <si>
+    <t>C_1103</t>
+  </si>
+  <si>
     <t>C_1148</t>
   </si>
   <si>
@@ -36,9 +39,18 @@
     <t>C_1119</t>
   </si>
   <si>
+    <t>C_1112</t>
+  </si>
+  <si>
+    <t>C_1110</t>
+  </si>
+  <si>
     <t>C_1155</t>
   </si>
   <si>
+    <t>C_1109</t>
+  </si>
+  <si>
     <t>C_1096</t>
   </si>
   <si>
@@ -48,6 +60,9 @@
     <t>C_1040</t>
   </si>
   <si>
+    <t>C_1089</t>
+  </si>
+  <si>
     <t>Nome</t>
   </si>
   <si>
@@ -60,6 +75,9 @@
     <t>ARNALDO TORRES</t>
   </si>
   <si>
+    <t>ELISA FILIPE</t>
+  </si>
+  <si>
     <t>FERNANDO JORGE</t>
   </si>
   <si>
@@ -69,9 +87,18 @@
     <t>GUERRA RAZAO</t>
   </si>
   <si>
+    <t>HELENA MANGUISE</t>
+  </si>
+  <si>
+    <t>ISABEL MATEUS</t>
+  </si>
+  <si>
     <t>JORGE MATEUS</t>
   </si>
   <si>
+    <t>LUCIA ZACARIAS</t>
+  </si>
+  <si>
     <t>MATEUS LUCAS KUMBI</t>
   </si>
   <si>
@@ -81,6 +108,9 @@
     <t>ROGERIO MERCIDO</t>
   </si>
   <si>
+    <t>ROSITA MANUEL</t>
+  </si>
+  <si>
     <t>Idade</t>
   </si>
   <si>
@@ -90,6 +120,9 @@
     <t>MASCULINO</t>
   </si>
   <si>
+    <t>FEMININO</t>
+  </si>
+  <si>
     <t>Comunidade</t>
   </si>
   <si>
@@ -114,7 +147,13 @@
     <t>H_1</t>
   </si>
   <si>
+    <t>AP-2</t>
+  </si>
+  <si>
     <t>AP-6</t>
+  </si>
+  <si>
+    <t>AP-1</t>
   </si>
   <si>
     <t>Membro_Influente</t>
@@ -218,7 +257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S16"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -226,58 +265,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="M1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="N1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="O1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="P1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="Q1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="R1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="S1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
@@ -285,54 +324,54 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0"/>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J2" s="0"/>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N2" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="P2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="Q2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="R2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -340,54 +379,54 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J3" s="0"/>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="P3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S3" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
@@ -395,54 +434,54 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="J4" s="0"/>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N4" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="P4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="Q4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R4" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="S4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5">
@@ -450,54 +489,54 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0"/>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J5" s="0"/>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="L5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N5" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="P5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="Q5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S5" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
@@ -505,54 +544,54 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="0"/>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J6" s="0"/>
       <c r="K6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N6" s="0">
         <v>8</v>
       </c>
       <c r="O6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="R6" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -560,54 +599,54 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0"/>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J7" s="0"/>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M7" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N7" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="P7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q7" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="R7" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
@@ -615,54 +654,54 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0"/>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J8" s="0"/>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M8" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N8" s="0">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="P8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="Q8" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="R8" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S8" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -670,54 +709,54 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0"/>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J9" s="0"/>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M9" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N9" s="0">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O9" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="P9" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="Q9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R9" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -725,54 +764,54 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C10" s="0"/>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="J10" s="0"/>
       <c r="K10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="L10" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="M10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N10" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="O10" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="P10" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="Q10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R10" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S10" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
@@ -780,54 +819,331 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C11" s="0"/>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="J11" s="0"/>
       <c r="K11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="L11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N11" s="0">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>48</v>
+      </c>
+      <c r="P11" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R11" t="s">
+        <v>64</v>
+      </c>
+      <c r="S11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="0"/>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="0"/>
+      <c r="K12" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="0">
         <v>7</v>
       </c>
-      <c r="O11" t="s">
-        <v>36</v>
-      </c>
-      <c r="P11" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="O12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" t="s">
+        <v>64</v>
+      </c>
+      <c r="S12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="0"/>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="0"/>
+      <c r="K13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="0">
+        <v>5</v>
+      </c>
+      <c r="O13" t="s">
+        <v>49</v>
+      </c>
+      <c r="P13" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" t="s">
+        <v>64</v>
+      </c>
+      <c r="S13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="0"/>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="0"/>
+      <c r="K14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="0">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R14" t="s">
+        <v>64</v>
+      </c>
+      <c r="S14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="0"/>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="0"/>
+      <c r="K15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="0">
+        <v>4</v>
+      </c>
+      <c r="O15" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>48</v>
+      </c>
+      <c r="R15" t="s">
+        <v>65</v>
+      </c>
+      <c r="S15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="0"/>
+      <c r="D16" t="s">
         <v>35</v>
       </c>
-      <c r="R11" t="s">
-        <v>52</v>
-      </c>
-      <c r="S11" t="s">
-        <v>35</v>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="0">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" t="s">
+        <v>48</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="0">
+        <v>2</v>
+      </c>
+      <c r="O16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>62</v>
+      </c>
+      <c r="R16" t="s">
+        <v>64</v>
+      </c>
+      <c r="S16" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>